<commit_message>
Update second sprint backlog
</commit_message>
<xml_diff>
--- a/docs/process/sprint-2-backlog.xlsx
+++ b/docs/process/sprint-2-backlog.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>Remaining effort at the end of the day ...</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>Artegiani, Tagliaferri</t>
+  </si>
+  <si>
+    <t>/</t>
   </si>
   <si>
     <t>Gestione architettura</t>
@@ -431,43 +434,66 @@
       <c r="D6" s="3">
         <v>3.0</v>
       </c>
-      <c r="E6" s="1"/>
+      <c r="E6" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="F6" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="G6" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D7" s="3">
         <v>2.0</v>
       </c>
-      <c r="E7" s="1"/>
+      <c r="E7" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="1"/>
       <c r="B8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="D8" s="3">
         <v>2.0</v>
       </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="E8" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="F8" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>10</v>

</xml_diff>